<commit_message>
Updated the Excel table tests and test data to include unicode testing.
</commit_message>
<xml_diff>
--- a/python-src/test/test_data/test_table-valid.xlsx
+++ b/python-src/test/test_data/test_table-valid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -32,12 +32,6 @@
     <t xml:space="preserve">  extra whitespace!  </t>
   </si>
   <si>
-    <t>the</t>
-  </si>
-  <si>
-    <t>last</t>
-  </si>
-  <si>
     <t>row</t>
   </si>
   <si>
@@ -48,6 +42,12 @@
   </si>
   <si>
     <t>one more</t>
+  </si>
+  <si>
+    <t>α</t>
+  </si>
+  <si>
+    <t>unicode</t>
   </si>
 </sst>
 </file>
@@ -59,7 +59,7 @@
     <numFmt numFmtId="165" formatCode="mmm\.\ d\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -69,6 +69,11 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -92,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -115,6 +120,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -482,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -518,14 +524,14 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -540,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -552,13 +558,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>